<commit_message>
curfew time is written to spreadsheet now as well, fixed countdown timer
</commit_message>
<xml_diff>
--- a/resources/files/test3.xlsx
+++ b/resources/files/test3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
   <si>
     <t>Bunk</t>
   </si>
@@ -218,10 +218,16 @@
     <t>SB1 Specialty Counselor 21</t>
   </si>
   <si>
+    <t>Curfew</t>
+  </si>
+  <si>
     <t>05/29/2020</t>
   </si>
   <si>
-    <t>TEST NAME</t>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>9:21 PM</t>
   </si>
   <si>
     <t>Shmira</t>
@@ -230,7 +236,16 @@
     <t>Day Off</t>
   </si>
   <si>
-    <t>6:47 PM</t>
+    <t>9:18 PM</t>
+  </si>
+  <si>
+    <t>9:20 PM</t>
+  </si>
+  <si>
+    <t>9:22 PM</t>
+  </si>
+  <si>
+    <t>9:30 PM</t>
   </si>
 </sst>
 </file>
@@ -552,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -582,19 +597,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -606,45 +609,19 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2.0</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -652,22 +629,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -675,22 +646,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E5" t="n">
         <v>2.0</v>
       </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
       <c r="F5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -698,42 +663,36 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
         <v>2.0</v>
       </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
       <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
         <v>1.0</v>
       </c>
-      <c r="E7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" t="s">
-        <v>5</v>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -741,19 +700,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="n">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
         <v>1.0</v>
       </c>
-      <c r="E8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" t="s">
-        <v>5</v>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -761,18 +720,15 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.0</v>
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" t="s">
+        <v>2.0</v>
+      </c>
+      <c r="F9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -781,38 +737,32 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1.0</v>
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" t="s">
+        <v>2.0</v>
+      </c>
+      <c r="F10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1.0</v>
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" t="s">
+        <v>2.0</v>
+      </c>
+      <c r="F11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -821,15 +771,15 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="E12" t="n">
         <v>2.0</v>
       </c>
-      <c r="H12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="F12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -838,15 +788,12 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E13" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13" t="s">
+        <v>3.0</v>
+      </c>
+      <c r="F13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -855,32 +802,26 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E14" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" t="s">
+        <v>3.0</v>
+      </c>
+      <c r="F14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J15" t="s">
+        <v>3.0</v>
+      </c>
+      <c r="F15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -889,390 +830,339 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>3.0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>3.0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
         <v>2.0</v>
       </c>
-      <c r="H18" t="s">
-        <v>5</v>
-      </c>
-      <c r="J18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>5</v>
-      </c>
-      <c r="J19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>66</v>
-      </c>
-      <c r="J20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="C21" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>66</v>
-      </c>
-      <c r="J21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
+      <c r="C22">
+        <v>1</v>
       </c>
       <c r="E22" t="n">
         <v>2.0</v>
       </c>
-      <c r="H22" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>35</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E24" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
         <v>2.0</v>
       </c>
-      <c r="H23" t="s">
-        <v>5</v>
-      </c>
-      <c r="J23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" t="n">
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
         <v>2.0</v>
       </c>
-      <c r="H24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>5</v>
-      </c>
-      <c r="J26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H28" t="s">
-        <v>5</v>
-      </c>
-      <c r="J28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H29" t="s">
-        <v>5</v>
-      </c>
-      <c r="J29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H30" t="s">
-        <v>5</v>
-      </c>
-      <c r="J30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H31" t="s">
-        <v>5</v>
-      </c>
-      <c r="J31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-      <c r="E32" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H32" t="s">
-        <v>5</v>
-      </c>
-      <c r="J32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H33" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H34" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
-      <c r="E35" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H35" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H36" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" t="s">
-        <v>63</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E37" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I37" t="s">
-        <v>66</v>
-      </c>
-      <c r="J37" t="s">
+      <c r="F38" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
allows for blank rows and columns now
</commit_message>
<xml_diff>
--- a/resources/files/test3.xlsx
+++ b/resources/files/test3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="74">
   <si>
     <t>Bunk</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Cooper</t>
   </si>
   <si>
-    <t>9:21 PM</t>
-  </si>
-  <si>
     <t>Shmira</t>
   </si>
   <si>
@@ -245,7 +242,10 @@
     <t>9:22 PM</t>
   </si>
   <si>
-    <t>9:30 PM</t>
+    <t>10:00 PM</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -282,8 +282,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -578,9 +581,12 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.89453125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="27.05078125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="8.83984375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.83984375" collapsed="false"/>
+    <col min="7" max="9" bestFit="true" customWidth="true" width="11.62890625" collapsed="false"/>
+    <col min="12" max="12" width="11.65625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,569 +599,724 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1"/>
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E4">
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="E9" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="E19" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
+      <c r="I22" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="E20" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+      <c r="I23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+      <c r="I24" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+      <c r="I25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K25" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="E23" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
+      <c r="I26" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="E24" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
+      <c r="I27" t="s">
+        <v>5</v>
+      </c>
+      <c r="K27" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="E25" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
+      <c r="I28" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>39</v>
       </c>
-      <c r="E26" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
+      <c r="I29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>41</v>
       </c>
-      <c r="E27" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
+      <c r="I30" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
         <v>42</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>43</v>
       </c>
-      <c r="E28" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
+      <c r="I31" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
         <v>44</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>45</v>
       </c>
-      <c r="E29" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
+      <c r="I32" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="E30" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
+      <c r="I33" t="s">
+        <v>5</v>
+      </c>
+      <c r="K33" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>49</v>
       </c>
-      <c r="E31" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
+      <c r="I34" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
         <v>50</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" t="s">
         <v>51</v>
       </c>
-      <c r="E32" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
+      <c r="I35" t="s">
+        <v>5</v>
+      </c>
+      <c r="K35" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>53</v>
       </c>
-      <c r="E33" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
+      <c r="I36" t="s">
+        <v>5</v>
+      </c>
+      <c r="K36" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
         <v>54</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="E34" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
+      <c r="I37" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
         <v>56</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>57</v>
       </c>
-      <c r="E35" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
+      <c r="I38" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
         <v>58</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>59</v>
       </c>
-      <c r="E36" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+      <c r="I39" t="s">
+        <v>5</v>
+      </c>
+      <c r="K39" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
         <v>60</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>61</v>
       </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
+      <c r="I40" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
         <v>62</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>63</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="I41" t="s">
+        <v>5</v>
+      </c>
+      <c r="K41" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="L41" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed Save And Quit button to Save and Return, moved Sign In button to right of idField
</commit_message>
<xml_diff>
--- a/resources/files/test3.xlsx
+++ b/resources/files/test3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17csc\eclipse-workspace\harlam-ozeret\resources\files\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="70">
   <si>
     <t>Bunk</t>
   </si>
@@ -219,12 +219,28 @@
   </si>
   <si>
     <t>Curfew</t>
+  </si>
+  <si>
+    <t>06/09/2020</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>1:11 AM</t>
+  </si>
+  <si>
+    <t>Shmira</t>
+  </si>
+  <si>
+    <t>3:32 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,7 +558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -550,11 +566,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.05078125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.05078125" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.83984375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.89453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.05078125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.05078125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="8.83984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.65625" collapsed="true"/>
+    <col min="8" max="8" width="11.65625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -573,6 +590,12 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
@@ -583,7 +606,12 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
@@ -594,7 +622,12 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -603,6 +636,15 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="F4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -611,6 +653,15 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="F5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -619,6 +670,15 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="F6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -627,6 +687,15 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
+      <c r="F7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
@@ -635,6 +704,15 @@
       <c r="B9" t="s">
         <v>13</v>
       </c>
+      <c r="F9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
@@ -643,6 +721,15 @@
       <c r="B10" t="s">
         <v>14</v>
       </c>
+      <c r="F10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
@@ -651,6 +738,15 @@
       <c r="B11" t="s">
         <v>17</v>
       </c>
+      <c r="F11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
@@ -659,6 +755,18 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
+      <c r="E12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
@@ -667,6 +775,15 @@
       <c r="B14" t="s">
         <v>18</v>
       </c>
+      <c r="F14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
@@ -675,6 +792,15 @@
       <c r="B15" t="s">
         <v>19</v>
       </c>
+      <c r="F15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
@@ -683,6 +809,15 @@
       <c r="B16" t="s">
         <v>15</v>
       </c>
+      <c r="F16" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
@@ -691,6 +826,15 @@
       <c r="B17" t="s">
         <v>20</v>
       </c>
+      <c r="F17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
@@ -699,6 +843,15 @@
       <c r="B19" t="s">
         <v>22</v>
       </c>
+      <c r="F19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
@@ -707,6 +860,15 @@
       <c r="B20" t="s">
         <v>23</v>
       </c>
+      <c r="F20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
@@ -715,6 +877,15 @@
       <c r="B21" t="s">
         <v>24</v>
       </c>
+      <c r="F21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
@@ -723,6 +894,15 @@
       <c r="B22" t="s">
         <v>25</v>
       </c>
+      <c r="F22" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
@@ -731,6 +911,18 @@
       <c r="B23" t="s">
         <v>31</v>
       </c>
+      <c r="D23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
@@ -739,6 +931,18 @@
       <c r="B24" t="s">
         <v>32</v>
       </c>
+      <c r="E24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
@@ -747,6 +951,15 @@
       <c r="B25" t="s">
         <v>33</v>
       </c>
+      <c r="F25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
@@ -755,6 +968,15 @@
       <c r="B26" t="s">
         <v>34</v>
       </c>
+      <c r="F26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
@@ -763,6 +985,15 @@
       <c r="B27" t="s">
         <v>35</v>
       </c>
+      <c r="F27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
@@ -771,6 +1002,15 @@
       <c r="B28" t="s">
         <v>37</v>
       </c>
+      <c r="F28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
@@ -779,6 +1019,15 @@
       <c r="B29" t="s">
         <v>39</v>
       </c>
+      <c r="F29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
@@ -787,6 +1036,15 @@
       <c r="B30" t="s">
         <v>41</v>
       </c>
+      <c r="F30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
@@ -795,6 +1053,15 @@
       <c r="B31" t="s">
         <v>43</v>
       </c>
+      <c r="F31" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
@@ -803,6 +1070,15 @@
       <c r="B32" t="s">
         <v>45</v>
       </c>
+      <c r="F32" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
@@ -811,6 +1087,15 @@
       <c r="B33" t="s">
         <v>47</v>
       </c>
+      <c r="F33" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
@@ -819,6 +1104,15 @@
       <c r="B34" t="s">
         <v>49</v>
       </c>
+      <c r="F34" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
@@ -827,6 +1121,15 @@
       <c r="B35" t="s">
         <v>51</v>
       </c>
+      <c r="F35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
@@ -835,6 +1138,15 @@
       <c r="B36" t="s">
         <v>53</v>
       </c>
+      <c r="F36" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
@@ -843,6 +1155,15 @@
       <c r="B37" t="s">
         <v>55</v>
       </c>
+      <c r="F37" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
@@ -851,6 +1172,15 @@
       <c r="B38" t="s">
         <v>57</v>
       </c>
+      <c r="F38" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
@@ -859,6 +1189,15 @@
       <c r="B39" t="s">
         <v>59</v>
       </c>
+      <c r="F39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
@@ -867,6 +1206,15 @@
       <c r="B40" t="s">
         <v>61</v>
       </c>
+      <c r="F40" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
@@ -874,6 +1222,15 @@
       </c>
       <c r="B41" t="s">
         <v>63</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>5</v>
+      </c>
+      <c r="H41" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unaccounted-for staff window now closes when returning to setup
</commit_message>
<xml_diff>
--- a/resources/files/test3.xlsx
+++ b/resources/files/test3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="70">
   <si>
     <t>Bunk</t>
   </si>
@@ -558,7 +558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
@@ -571,7 +571,9 @@
     <col min="3" max="3" customWidth="true" width="27.05078125" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="8.83984375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="11.65625" collapsed="true"/>
-    <col min="8" max="8" width="11.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.65625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.65625" collapsed="false"/>
+    <col min="10" max="10" width="11.65625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -594,6 +596,12 @@
         <v>65</v>
       </c>
       <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -612,6 +620,12 @@
       <c r="H2" t="s">
         <v>66</v>
       </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
@@ -628,6 +642,12 @@
       <c r="H3" t="s">
         <v>67</v>
       </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -637,12 +657,18 @@
         <v>8</v>
       </c>
       <c r="F4" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G4" t="s">
         <v>5</v>
       </c>
       <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -654,12 +680,18 @@
         <v>9</v>
       </c>
       <c r="F5" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -671,12 +703,18 @@
         <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -688,12 +726,18 @@
         <v>11</v>
       </c>
       <c r="F7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
       <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -705,12 +749,18 @@
         <v>13</v>
       </c>
       <c r="F9" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -722,12 +772,18 @@
         <v>14</v>
       </c>
       <c r="F10" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G10" t="s">
         <v>5</v>
       </c>
       <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -739,12 +795,18 @@
         <v>17</v>
       </c>
       <c r="F11" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G11" t="s">
         <v>5</v>
       </c>
       <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -759,12 +821,18 @@
         <v>1.0</v>
       </c>
       <c r="F12" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G12" t="s">
         <v>69</v>
       </c>
       <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -776,12 +844,18 @@
         <v>18</v>
       </c>
       <c r="F14" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G14" t="s">
         <v>5</v>
       </c>
       <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -793,12 +867,18 @@
         <v>19</v>
       </c>
       <c r="F15" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
       <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -810,12 +890,18 @@
         <v>15</v>
       </c>
       <c r="F16" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G16" t="s">
         <v>5</v>
       </c>
       <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
         <v>5</v>
       </c>
     </row>
@@ -827,12 +913,18 @@
         <v>20</v>
       </c>
       <c r="F17" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
       </c>
       <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -844,12 +936,18 @@
         <v>22</v>
       </c>
       <c r="F19" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
       </c>
       <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -861,12 +959,18 @@
         <v>23</v>
       </c>
       <c r="F20" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G20" t="s">
         <v>5</v>
       </c>
       <c r="H20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -878,12 +982,18 @@
         <v>24</v>
       </c>
       <c r="F21" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G21" t="s">
         <v>5</v>
       </c>
       <c r="H21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" t="s">
         <v>5</v>
       </c>
     </row>
@@ -895,12 +1005,18 @@
         <v>25</v>
       </c>
       <c r="F22" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
       <c r="H22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" t="s">
         <v>5</v>
       </c>
     </row>
@@ -915,12 +1031,18 @@
         <v>1.0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G23" t="s">
         <v>68</v>
       </c>
       <c r="H23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -935,12 +1057,18 @@
         <v>1.0</v>
       </c>
       <c r="F24" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G24" t="s">
         <v>69</v>
       </c>
       <c r="H24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" t="s">
         <v>5</v>
       </c>
     </row>
@@ -952,12 +1080,18 @@
         <v>33</v>
       </c>
       <c r="F25" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
       <c r="H25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" t="s">
         <v>5</v>
       </c>
     </row>
@@ -969,12 +1103,18 @@
         <v>34</v>
       </c>
       <c r="F26" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G26" t="s">
         <v>5</v>
       </c>
       <c r="H26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" t="s">
         <v>5</v>
       </c>
     </row>
@@ -986,12 +1126,18 @@
         <v>35</v>
       </c>
       <c r="F27" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G27" t="s">
         <v>5</v>
       </c>
       <c r="H27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1003,12 +1149,18 @@
         <v>37</v>
       </c>
       <c r="F28" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
       <c r="H28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1020,12 +1172,18 @@
         <v>39</v>
       </c>
       <c r="F29" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G29" t="s">
         <v>5</v>
       </c>
       <c r="H29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1037,12 +1195,18 @@
         <v>41</v>
       </c>
       <c r="F30" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G30" t="s">
         <v>5</v>
       </c>
       <c r="H30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1054,12 +1218,18 @@
         <v>43</v>
       </c>
       <c r="F31" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G31" t="s">
         <v>5</v>
       </c>
       <c r="H31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" t="s">
+        <v>5</v>
+      </c>
+      <c r="J31" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1071,12 +1241,18 @@
         <v>45</v>
       </c>
       <c r="F32" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G32" t="s">
         <v>5</v>
       </c>
       <c r="H32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1088,12 +1264,18 @@
         <v>47</v>
       </c>
       <c r="F33" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G33" t="s">
         <v>5</v>
       </c>
       <c r="H33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1105,12 +1287,18 @@
         <v>49</v>
       </c>
       <c r="F34" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G34" t="s">
         <v>5</v>
       </c>
       <c r="H34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1122,12 +1310,18 @@
         <v>51</v>
       </c>
       <c r="F35" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G35" t="s">
         <v>5</v>
       </c>
       <c r="H35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1139,12 +1333,18 @@
         <v>53</v>
       </c>
       <c r="F36" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
       <c r="H36" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1156,12 +1356,18 @@
         <v>55</v>
       </c>
       <c r="F37" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G37" t="s">
         <v>5</v>
       </c>
       <c r="H37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1173,12 +1379,18 @@
         <v>57</v>
       </c>
       <c r="F38" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G38" t="s">
         <v>5</v>
       </c>
       <c r="H38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1190,12 +1402,18 @@
         <v>59</v>
       </c>
       <c r="F39" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G39" t="s">
         <v>5</v>
       </c>
       <c r="H39" t="s">
+        <v>5</v>
+      </c>
+      <c r="I39" t="s">
+        <v>5</v>
+      </c>
+      <c r="J39" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1207,12 +1425,18 @@
         <v>61</v>
       </c>
       <c r="F40" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G40" t="s">
         <v>5</v>
       </c>
       <c r="H40" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1224,12 +1448,18 @@
         <v>63</v>
       </c>
       <c r="F41" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G41" t="s">
         <v>5</v>
       </c>
       <c r="H41" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added standalone folder to this repository, updated README.md, added LICENSE, NOTICE
</commit_message>
<xml_diff>
--- a/resources/files/test3.xlsx
+++ b/resources/files/test3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17csc\eclipse-workspace\harlam-ozeret\resources\files\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>Bunk</t>
   </si>
@@ -219,28 +219,12 @@
   </si>
   <si>
     <t>Curfew</t>
-  </si>
-  <si>
-    <t>06/09/2020</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>1:11 AM</t>
-  </si>
-  <si>
-    <t>Shmira</t>
-  </si>
-  <si>
-    <t>3:32 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,11 +254,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -558,25 +539,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.89453125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.05078125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="27.05078125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="8.83984375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.65625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.65625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.65625" collapsed="false"/>
-    <col min="10" max="10" width="11.65625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.05078125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.05078125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.83984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,317 +569,113 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="F15" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
-      </c>
-      <c r="F16" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -912,21 +685,6 @@
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
@@ -935,21 +693,6 @@
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" t="s">
-        <v>5</v>
-      </c>
-      <c r="J19" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
@@ -958,21 +701,6 @@
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="F20" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" t="s">
-        <v>5</v>
-      </c>
-      <c r="I20" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
@@ -981,21 +709,6 @@
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="F21" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" t="s">
-        <v>5</v>
-      </c>
-      <c r="I21" t="s">
-        <v>5</v>
-      </c>
-      <c r="J21" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
@@ -1004,21 +717,6 @@
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G22" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
@@ -1027,24 +725,6 @@
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="D23" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F23" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="G23" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" t="s">
-        <v>5</v>
-      </c>
-      <c r="J23" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
@@ -1053,24 +733,6 @@
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="E24" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="G24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
@@ -1079,21 +741,6 @@
       <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="F25" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" t="s">
-        <v>5</v>
-      </c>
-      <c r="I25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J25" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
@@ -1102,21 +749,6 @@
       <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="F26" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" t="s">
-        <v>5</v>
-      </c>
-      <c r="I26" t="s">
-        <v>5</v>
-      </c>
-      <c r="J26" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
@@ -1125,21 +757,6 @@
       <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="F27" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G27" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J27" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
@@ -1148,21 +765,6 @@
       <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="F28" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G28" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" t="s">
-        <v>5</v>
-      </c>
-      <c r="J28" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
@@ -1171,21 +773,6 @@
       <c r="B29" t="s">
         <v>39</v>
       </c>
-      <c r="F29" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G29" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" t="s">
-        <v>5</v>
-      </c>
-      <c r="I29" t="s">
-        <v>5</v>
-      </c>
-      <c r="J29" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
@@ -1194,21 +781,6 @@
       <c r="B30" t="s">
         <v>41</v>
       </c>
-      <c r="F30" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G30" t="s">
-        <v>5</v>
-      </c>
-      <c r="H30" t="s">
-        <v>5</v>
-      </c>
-      <c r="I30" t="s">
-        <v>5</v>
-      </c>
-      <c r="J30" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
@@ -1217,21 +789,6 @@
       <c r="B31" t="s">
         <v>43</v>
       </c>
-      <c r="F31" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G31" t="s">
-        <v>5</v>
-      </c>
-      <c r="H31" t="s">
-        <v>5</v>
-      </c>
-      <c r="I31" t="s">
-        <v>5</v>
-      </c>
-      <c r="J31" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
@@ -1240,21 +797,6 @@
       <c r="B32" t="s">
         <v>45</v>
       </c>
-      <c r="F32" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G32" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" t="s">
-        <v>5</v>
-      </c>
-      <c r="J32" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
@@ -1263,21 +805,6 @@
       <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="F33" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
@@ -1286,21 +813,6 @@
       <c r="B34" t="s">
         <v>49</v>
       </c>
-      <c r="F34" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G34" t="s">
-        <v>5</v>
-      </c>
-      <c r="H34" t="s">
-        <v>5</v>
-      </c>
-      <c r="I34" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
@@ -1309,21 +821,6 @@
       <c r="B35" t="s">
         <v>51</v>
       </c>
-      <c r="F35" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G35" t="s">
-        <v>5</v>
-      </c>
-      <c r="H35" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
@@ -1332,21 +829,6 @@
       <c r="B36" t="s">
         <v>53</v>
       </c>
-      <c r="F36" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G36" t="s">
-        <v>5</v>
-      </c>
-      <c r="H36" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
@@ -1355,21 +837,6 @@
       <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="F37" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G37" t="s">
-        <v>5</v>
-      </c>
-      <c r="H37" t="s">
-        <v>5</v>
-      </c>
-      <c r="I37" t="s">
-        <v>5</v>
-      </c>
-      <c r="J37" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
@@ -1378,21 +845,6 @@
       <c r="B38" t="s">
         <v>57</v>
       </c>
-      <c r="F38" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G38" t="s">
-        <v>5</v>
-      </c>
-      <c r="H38" t="s">
-        <v>5</v>
-      </c>
-      <c r="I38" t="s">
-        <v>5</v>
-      </c>
-      <c r="J38" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
@@ -1401,21 +853,6 @@
       <c r="B39" t="s">
         <v>59</v>
       </c>
-      <c r="F39" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G39" t="s">
-        <v>5</v>
-      </c>
-      <c r="H39" t="s">
-        <v>5</v>
-      </c>
-      <c r="I39" t="s">
-        <v>5</v>
-      </c>
-      <c r="J39" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
@@ -1424,21 +861,6 @@
       <c r="B40" t="s">
         <v>61</v>
       </c>
-      <c r="F40" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" t="s">
-        <v>5</v>
-      </c>
-      <c r="I40" t="s">
-        <v>5</v>
-      </c>
-      <c r="J40" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
@@ -1446,21 +868,6 @@
       </c>
       <c r="B41" t="s">
         <v>63</v>
-      </c>
-      <c r="F41" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="G41" t="s">
-        <v>5</v>
-      </c>
-      <c r="H41" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" t="s">
-        <v>5</v>
-      </c>
-      <c r="J41" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a bug where the clock text would be unreadable if restarting from setup. added cell coloring based on sign-in time
</commit_message>
<xml_diff>
--- a/resources/files/test3.xlsx
+++ b/resources/files/test3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Bunk</t>
   </si>
@@ -113,12 +113,6 @@
     <t>Sharon Boys 4</t>
   </si>
   <si>
-    <t>Sharon Boys 5</t>
-  </si>
-  <si>
-    <t>Sharon Boys 6</t>
-  </si>
-  <si>
     <t>SB1 Specialty Counselor 3</t>
   </si>
   <si>
@@ -126,96 +120,6 @@
   </si>
   <si>
     <t>SB1 Specialty Counselor 5</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 6</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 7</t>
-  </si>
-  <si>
-    <t>Sharon Boys 7</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 8</t>
-  </si>
-  <si>
-    <t>Sharon Boys 8</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 9</t>
-  </si>
-  <si>
-    <t>Sharon Boys 9</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 10</t>
-  </si>
-  <si>
-    <t>Sharon Boys 10</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 11</t>
-  </si>
-  <si>
-    <t>Sharon Boys 11</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 12</t>
-  </si>
-  <si>
-    <t>Sharon Boys 12</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 13</t>
-  </si>
-  <si>
-    <t>Sharon Boys 13</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 14</t>
-  </si>
-  <si>
-    <t>Sharon Boys 14</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 15</t>
-  </si>
-  <si>
-    <t>Sharon Boys 15</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 16</t>
-  </si>
-  <si>
-    <t>Sharon Boys 16</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 17</t>
-  </si>
-  <si>
-    <t>Sharon Boys 17</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 18</t>
-  </si>
-  <si>
-    <t>Sharon Boys 18</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 19</t>
-  </si>
-  <si>
-    <t>Sharon Boys 19</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 20</t>
-  </si>
-  <si>
-    <t>Sharon Boys 20</t>
-  </si>
-  <si>
-    <t>SB1 Specialty Counselor 21</t>
   </si>
   <si>
     <t>Curfew</t>
@@ -539,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D4" sqref="D4:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -550,7 +454,6 @@
     <col min="1" max="1" width="11.89453125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27.05078125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="27.05078125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -582,7 +485,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -723,7 +626,7 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -731,7 +634,7 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -739,135 +642,7 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>58</v>
-      </c>
-      <c r="B39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>